<commit_message>
Fixed ADCP cal files for GA-3 and GS-3
- CC_depth provided was water depth. Updated to ADCP deployment depth
- fixed values in archived deployment sheets
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_GS03FLMA_00003.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_GS03FLMA_00003.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1"/>
+    <workbookView xWindow="-1400" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -946,7 +946,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1091,6 +1091,9 @@
     </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="210">
@@ -1736,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" workbookViewId="0">
-      <selection activeCell="J375" sqref="J375"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2490,8 +2493,8 @@
       <c r="G29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="11">
-        <v>4627000</v>
+      <c r="H29" s="49">
+        <v>500000</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>48</v>

</xml_diff>